<commit_message>
add bg, change favicon
</commit_message>
<xml_diff>
--- a/static/quiz.xlsx
+++ b/static/quiz.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="136">
   <si>
     <t>题目</t>
   </si>
@@ -263,60 +263,57 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">打印机
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">B.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">数据库
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">C.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">磁盘
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">D.</t>
+      <t xml:space="preserve">打印机</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">;B.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">数据库</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">;C.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">磁盘</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">;D.</t>
     </r>
     <r>
       <rPr>
@@ -416,6 +413,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">科学计算</t>
     </r>
@@ -435,6 +433,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">实时控制</t>
     </r>
@@ -454,6 +453,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">数据处理</t>
     </r>
@@ -473,6 +473,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">人工智能 </t>
     </r>
@@ -526,6 +527,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">最左边一位为</t>
     </r>
@@ -545,6 +547,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">最右边一位为</t>
     </r>
@@ -564,6 +567,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">最左边一位为</t>
     </r>
@@ -583,6 +587,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">最右边一位为</t>
     </r>
@@ -634,6 +639,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">模拟计算机</t>
     </r>
@@ -653,6 +659,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">通用并专门用于家庭的计算机</t>
     </r>
@@ -672,6 +679,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">数字与模拟混合的计算机</t>
     </r>
@@ -691,6 +699,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">数字计算机</t>
     </r>
@@ -729,6 +738,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">喷墨打印机</t>
     </r>
@@ -748,6 +758,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">显示器</t>
     </r>
@@ -767,6 +778,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">键盘</t>
     </r>
@@ -786,6 +798,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">激光打印机，键盘，鼠标器</t>
     </r>
@@ -805,6 +818,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">键盘，鼠标器，扫描仪</t>
     </r>
@@ -824,6 +838,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">打印机，绘图仪，显示器</t>
     </r>
@@ -841,6 +856,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">计算机程序、数据与相应文档的总称</t>
     </r>
@@ -860,6 +876,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">系统软件与应用软件的总和</t>
     </r>
@@ -879,6 +896,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">操作系统、数据库管理软件与应用软件的总和</t>
     </r>
@@ -898,6 +916,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">各类应用软件的总称 </t>
     </r>
@@ -915,6 +934,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">倍</t>
     </r>
@@ -934,6 +954,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">倍</t>
     </r>
@@ -953,6 +974,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">倍</t>
     </r>
@@ -972,6 +994,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">倍 </t>
     </r>
@@ -989,6 +1012,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">计算机能直接执行</t>
     </r>
@@ -1008,6 +1032,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">具有良好的可读性和可移植性</t>
     </r>
@@ -1027,6 +1052,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">执行效率高</t>
     </r>
@@ -1046,6 +1072,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">依赖于具体机器 </t>
     </r>
@@ -1063,6 +1090,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">资源共享和快速传输信息</t>
     </r>
@@ -1082,6 +1110,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">高精度计算和收发邮件</t>
     </r>
@@ -1101,6 +1130,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">运算速度快和快速传输信息</t>
     </r>
@@ -1120,6 +1150,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">存储容量大和高精度</t>
     </r>
@@ -1137,6 +1168,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">数据</t>
     </r>
@@ -1156,6 +1188,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">字符</t>
     </r>
@@ -1175,6 +1208,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">操作码</t>
     </r>
@@ -1194,6 +1228,7 @@
         <color rgb="FF000000"/>
         <rFont val="Droid Sans Fallback"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">地址码</t>
     </r>
@@ -1209,16 +1244,905 @@
   </si>
   <si>
     <t>Windows Vista属于系统软件?</t>
+  </si>
+  <si>
+    <t>中国国防科技大学研制的“银河”计算机属于</t>
+  </si>
+  <si>
+    <t>超级计算机</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">将二进制数</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1101101110</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">转换为八进制数是</t>
+    </r>
+  </si>
+  <si>
+    <t>进制</t>
+  </si>
+  <si>
+    <t>一个汉字的国标码可以用两个字节存储，这两个字节的最高位分别是</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">和</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1;B.O</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">和</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">0;C.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">和</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">O;D.0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">和</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+  </si>
+  <si>
+    <t>编码</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">执行逻辑或表达式</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1010 V 1101</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">后，结果是</t>
+    </r>
+  </si>
+  <si>
+    <t>A.1010;B.1100;C.1011;D.11ll </t>
+  </si>
+  <si>
+    <t>逻辑</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">英文小写字母“</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">b”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">和大写字母“</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">B”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">的十六进制</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ASCII</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">码值相差多少？</t>
+    </r>
+  </si>
+  <si>
+    <t>20H</t>
+  </si>
+  <si>
+    <t>汉字系统中的汉字字库里存放的是什么？</t>
+  </si>
+  <si>
+    <t>汉字的字模</t>
+  </si>
+  <si>
+    <t>一个汉字和一个英文字符在微机中存储时所占字节数的比值为多少？</t>
+  </si>
+  <si>
+    <t>2:1 </t>
+  </si>
+  <si>
+    <t>计算机存储</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">计算机中的兼容是指计算机部件的通用性，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">IBM PC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">兼容机中的兼容是指在兼容机上可以使用什么类型的软件和设备？</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">与</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">IBM PC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">原型机上不同的软件和外部设备</t>
+    </r>
+  </si>
+  <si>
+    <t>通用计算机</t>
+  </si>
+  <si>
+    <t>将程序像数据一样存放在计算机内存中运行，是谁在哪一年提出的？</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">冯</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">诺依曼，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1946</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">年</t>
+    </r>
+  </si>
+  <si>
+    <t>在计算机系统中，指挥、协调计算机工作的设备是什么？</t>
+  </si>
+  <si>
+    <t>控制器</t>
+  </si>
+  <si>
+    <t>微处理器研制成功是在什么时候？</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1917</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">年</t>
+    </r>
+  </si>
+  <si>
+    <t>计算机文化</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CAD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">是计算机主要应用领域之一，其含义是什么？</t>
+    </r>
+  </si>
+  <si>
+    <t>计算机辅助设计</t>
+  </si>
+  <si>
+    <t>微型计算机的主要技术指标有哪些？</t>
+  </si>
+  <si>
+    <t>内存容量、字长和速度</t>
+  </si>
+  <si>
+    <t>在计算机运算过程中“溢出”一般是指什么？</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">是指计算机在运算过程中产生的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">数超过了机器的位所表示的范围</t>
+    </r>
+  </si>
+  <si>
+    <t>现代计算机是一种按程序自动进行信息处理的工具，目前被广泛使用的是哪种计算机？</t>
+  </si>
+  <si>
+    <t>数字与模拟混合的计算机</t>
+  </si>
+  <si>
+    <t>现代计算机</t>
+  </si>
+  <si>
+    <t>负数的补码怎么求？</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">先对原码中除符号位以外的各位求反，然后末位加</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+  </si>
+  <si>
+    <t>补码</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">在</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">24 x 24</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">点阵字库中，每个汉字的字模信息需用</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">72</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">个字节存储</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">用补码表示的、带符号的八位二进制数，可表示的整数范围是</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-127</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">～</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">+127</t>
+    </r>
+  </si>
+  <si>
+    <t>机器指令是用二进制代码表示的，能被计算机编译后执行</t>
+  </si>
+  <si>
+    <t>计算机指令系统主要包括数据处理指令、数据传送指令、程序控制指令和状态管理指令</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">汉字的机内码高位等于</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">( )</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">与</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">( )</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">之和</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">数字码</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">;B.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">位码</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">;C.AOH;D.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">区码 </t>
+    </r>
+  </si>
+  <si>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>下列属于多媒体计算机硬件系统的是   </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">摄像机</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">;B.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">音箱</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">;C.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">键盘</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">;D.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">操纵杆</t>
+    </r>
+  </si>
+  <si>
+    <t>ABCD</t>
+  </si>
+  <si>
+    <t>下列哪些是多媒体技术的特征</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">集成性</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">;B.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">交互性</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">;C.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">高速性</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">;D.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">实时性</t>
+    </r>
+  </si>
+  <si>
+    <t>多媒体基础</t>
+  </si>
+  <si>
+    <t>下列属于存储信息的实体的是</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">磁带</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">;B.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">磁盘</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">;C.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">光盘</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">;D.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">半导体存储器</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="H:MM"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1252,24 +2176,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Droid Sans Fallback"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="DejaVu Sans"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="DejaVu Sans"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1315,7 +2221,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1336,6 +2242,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1348,574 +2258,28 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>301680</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>4320</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>604800</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>12600</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="0" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15319080" y="4982040"/>
-          <a:ext cx="2604600" cy="522360"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeRoundRectCallout">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val -20114"/>
-            <a:gd name="adj2" fmla="val 101223"/>
-            <a:gd name="adj3" fmla="val 16667"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="d99694"/>
-        </a:solidFill>
-        <a:ln w="25560">
-          <a:solidFill>
-            <a:srgbClr val="3a5f8b"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000"/>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>这里要选择</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>Sheet1</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>，请保持默认不要修改</a:t>
-          </a:r>
-          <a:endParaRPr/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>336600</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>100080</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>316080</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>241920</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13052880" y="100080"/>
-          <a:ext cx="3047760" cy="1341720"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 16667"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="d99694"/>
-        </a:solidFill>
-        <a:ln w="25560">
-          <a:solidFill>
-            <a:srgbClr val="3a5f8b"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000"/>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>选择题选项以</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>A,B,C...</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>开头，后跟一个</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>'.'</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>（</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="ff0000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>必须有而且是英文符号</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>），选项之间以</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>';'</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>（</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="ff0000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>注意是英文符号</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>）或换行隔开，</a:t>
-          </a:r>
-          <a:endParaRPr/>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>判断题和问答题</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="ff0000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>请不要填写</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>选项一栏</a:t>
-          </a:r>
-          <a:endParaRPr/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>574920</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>375480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>459360</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>70200</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14058360" y="3471480"/>
-          <a:ext cx="2185560" cy="1062000"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 16667"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="d99694"/>
-        </a:solidFill>
-        <a:ln w="25560">
-          <a:solidFill>
-            <a:srgbClr val="3a5f8b"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000"/>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>选择题参考答案为</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>A,B,C...</a:t>
-          </a:r>
-          <a:endParaRPr/>
-        </a:p>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>答案之间</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="ff0000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>没有空隙</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>，判断题参考答案只能为</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>'</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="ff0000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>正确</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>'</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>和</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>'</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="ff0000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>错误</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>'</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>两种，问答题不限</a:t>
-          </a:r>
-          <a:endParaRPr/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>165240</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>1138680</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>50040</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>51480</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13648680" y="2338560"/>
-          <a:ext cx="2185920" cy="808920"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 16667"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="d99694"/>
-        </a:solidFill>
-        <a:ln w="25560">
-          <a:solidFill>
-            <a:srgbClr val="3a5f8b"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000"/>
-        <a:p>
-          <a:pPr>
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>题目对应知识点</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="ff0000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>必须填写</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>，且必须</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="ff0000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>对应当前章节</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>所有的，否则不能录入</a:t>
-          </a:r>
-          <a:endParaRPr/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E60" activeCellId="0" sqref="E60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.62753036437247"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.1255060728745"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.5546558704453"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.331983805668"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.1133603238866"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.004048582996"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.1255060728745"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.62753036437247"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.1093117408907"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.66396761133603"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1932,7 +2296,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1946,7 +2310,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1960,7 +2324,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1977,7 +2341,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -1994,7 +2358,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -2011,7 +2375,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -2028,7 +2392,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -2042,7 +2406,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="53.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -2056,7 +2420,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -2073,7 +2437,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -2090,7 +2454,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>35</v>
       </c>
@@ -2107,7 +2471,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -2124,7 +2488,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>39</v>
       </c>
@@ -2141,7 +2505,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
@@ -2158,49 +2522,49 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>47</v>
       </c>
@@ -2217,7 +2581,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>50</v>
       </c>
@@ -2234,7 +2598,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>53</v>
       </c>
@@ -2251,7 +2615,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>55</v>
       </c>
@@ -2268,7 +2632,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>57</v>
       </c>
@@ -2285,49 +2649,49 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>63</v>
       </c>
@@ -2344,7 +2708,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>66</v>
       </c>
@@ -2361,7 +2725,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>68</v>
       </c>
@@ -2378,7 +2742,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>70</v>
       </c>
@@ -2395,7 +2759,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
@@ -2412,7 +2776,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>74</v>
       </c>
@@ -2429,7 +2793,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>76</v>
       </c>
@@ -2446,46 +2810,400 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -2496,6 +3214,5 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>